<commit_message>
Fixed 5.4.3 lab sheet.
</commit_message>
<xml_diff>
--- a/5.4.3/Dedkov_Maslov/data/5.4.3.xlsx
+++ b/5.4.3/Dedkov_Maslov/data/5.4.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\mipt_lab\5.4.3\Dedkov_Maslov\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F492AE02-31E4-4FB0-AB3D-437F61FEA2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234E9EA-2C95-4B7F-9C10-D1887F796EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3756" yWindow="1380" windowWidth="14712" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5616" yWindow="1992" windowWidth="14712" windowHeight="9288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -612,8 +612,8 @@
         <v>33.774999999999999</v>
       </c>
       <c r="D3" s="1">
-        <f>SQRT(C3)/SQRT(A3)</f>
-        <v>4.1094403511913882</v>
+        <f>C3/SQRT(B3)</f>
+        <v>0.53052646807990012</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -626,8 +626,8 @@
         <v>27.033333333333335</v>
       </c>
       <c r="H3" s="1">
-        <f>SQRT(G3)/SQRT(E3)</f>
-        <v>3.6765019606504588</v>
+        <f>G3/SQRT(F3)</f>
+        <v>0.47463436219660476</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -640,8 +640,8 @@
         <v>2759.45</v>
       </c>
       <c r="M3" s="1">
-        <f>SQRT(L3)/SQRT(J3)</f>
-        <v>52.530467349910374</v>
+        <f>L3/SQRT(K3)</f>
+        <v>6.7816541738231777</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
@@ -654,8 +654,8 @@
         <v>1054.6333333333334</v>
       </c>
       <c r="Q3" s="1">
-        <f>SQRT(P3)/SQRT(N3)</f>
-        <v>32.475118680819833</v>
+        <f>P3/SQRT(O3)</f>
+        <v>4.1925197938974863</v>
       </c>
       <c r="S3" s="1">
         <v>0.2</v>
@@ -671,8 +671,8 @@
         <v>2</v>
       </c>
       <c r="W3" s="1">
-        <f>SQRT(V3)/SQRT(T3)</f>
-        <v>0.63245553203367588</v>
+        <f>V3/SQRT(U3)</f>
+        <v>8.1649658092772609E-2</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
@@ -687,8 +687,8 @@
         <v>33.575000000000003</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D5" si="1">SQRT(C4)/SQRT(A4)</f>
-        <v>4.0972551787751756</v>
+        <f t="shared" ref="D4:D5" si="1">C4/SQRT(B4)</f>
+        <v>0.52895336908527835</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -701,8 +701,8 @@
         <v>27.341666666666665</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H5" si="3">SQRT(G4)/SQRT(E4)</f>
-        <v>3.6974090027116731</v>
+        <f t="shared" ref="H4:H5" si="3">G4/SQRT(F4)</f>
+        <v>0.47733344972065622</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -715,8 +715,8 @@
         <v>2734.6666666666665</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:M6" si="5">SQRT(L4)/SQRT(J4)</f>
-        <v>52.294040450769018</v>
+        <f t="shared" ref="M4:M6" si="5">L4/SQRT(K4)</f>
+        <v>6.7511315923908466</v>
       </c>
       <c r="N4" s="1">
         <v>1</v>
@@ -729,8 +729,8 @@
         <v>1003.95</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" ref="Q4:Q6" si="7">SQRT(P4)/SQRT(N4)</f>
-        <v>31.685170032682482</v>
+        <f t="shared" ref="Q4:Q6" si="7">P4/SQRT(O4)</f>
+        <v>4.0905378619443189</v>
       </c>
       <c r="S4" s="1">
         <v>0.2</v>
@@ -746,8 +746,8 @@
         <v>1.9466666666666668</v>
       </c>
       <c r="W4" s="1">
-        <f>SQRT(V4)/SQRT(T4)</f>
-        <v>0.62396581102920479</v>
+        <f t="shared" ref="W4:W8" si="8">V4/SQRT(U4)</f>
+        <v>8.055363982396381E-2</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>4.1357183978925196</v>
+        <v>0.53391894932137818</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -777,7 +777,7 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="3"/>
-        <v>3.6651512019742558</v>
+        <v>0.473168985552613</v>
       </c>
       <c r="J5" s="1">
         <v>1</v>
@@ -791,7 +791,7 @@
       </c>
       <c r="M5" s="1">
         <f t="shared" si="5"/>
-        <v>52.212865592048608</v>
+        <v>6.7406519631923505</v>
       </c>
       <c r="N5" s="1">
         <v>1</v>
@@ -805,7 +805,7 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="7"/>
-        <v>31.54573399579305</v>
+        <v>4.072536746986521</v>
       </c>
       <c r="S5" s="1">
         <v>0.5</v>
@@ -817,12 +817,12 @@
         <v>609</v>
       </c>
       <c r="V5" s="1">
-        <f t="shared" ref="V5:V8" si="8">U5/(T5*60)</f>
+        <f t="shared" ref="V5:V8" si="9">U5/(T5*60)</f>
         <v>3.3833333333333333</v>
       </c>
       <c r="W5" s="1">
-        <f t="shared" ref="W5:W8" si="9">SQRT(V5)/SQRT(T5)</f>
-        <v>1.0619688214715994</v>
+        <f t="shared" si="8"/>
+        <v>0.13709958532503405</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
       </c>
       <c r="M6" s="1">
         <f t="shared" si="5"/>
-        <v>52.296749420972617</v>
+        <v>6.7514813189403107</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
@@ -852,7 +852,7 @@
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="7"/>
-        <v>31.640427725722461</v>
+        <v>4.0847616549534171</v>
       </c>
       <c r="S6" s="1">
         <v>0.5</v>
@@ -864,12 +864,12 @@
         <v>1075</v>
       </c>
       <c r="V6" s="1">
+        <f t="shared" si="9"/>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="W6" s="1">
         <f t="shared" si="8"/>
-        <v>3.5833333333333335</v>
-      </c>
-      <c r="W6" s="1">
-        <f t="shared" si="9"/>
-        <v>0.84656167328001952</v>
+        <v>0.10929064207170001</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -883,12 +883,12 @@
         <v>608</v>
       </c>
       <c r="V7" s="1">
+        <f t="shared" si="9"/>
+        <v>5.0666666666666664</v>
+      </c>
+      <c r="W7" s="1">
         <f t="shared" si="8"/>
-        <v>5.0666666666666664</v>
-      </c>
-      <c r="W7" s="1">
-        <f t="shared" si="9"/>
-        <v>1.5916448515084429</v>
+        <v>0.20548046676563256</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -902,12 +902,12 @@
         <v>645</v>
       </c>
       <c r="V8" s="1">
+        <f t="shared" si="9"/>
+        <v>5.375</v>
+      </c>
+      <c r="W8" s="1">
         <f t="shared" si="8"/>
-        <v>5.375</v>
-      </c>
-      <c r="W8" s="1">
-        <f t="shared" si="9"/>
-        <v>1.6393596310755001</v>
+        <v>0.21164041832000491</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>